<commit_message>
- Templates actualizados al 20200729_1030
</commit_message>
<xml_diff>
--- a/Template/Export/Sari_R5_11.xlsx
+++ b/Template/Export/Sari_R5_11.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20700" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20700" windowHeight="11760" tabRatio="662"/>
   </bookViews>
   <sheets>
     <sheet name="Global epidemiological week" sheetId="3" r:id="rId1"/>
@@ -19,13 +19,15 @@
     <sheet name="Inf A" sheetId="6" r:id="rId5"/>
     <sheet name="Inf B" sheetId="5" r:id="rId6"/>
     <sheet name="Metapnemovirus" sheetId="9" r:id="rId7"/>
+    <sheet name="SARS-CoV-2" sheetId="10" r:id="rId8"/>
+    <sheet name="Parameters" sheetId="11" state="hidden" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="43">
   <si>
     <t>Ad</t>
   </si>
@@ -98,12 +100,69 @@
   <si>
     <t>AÑO EPIDEM.</t>
   </si>
+  <si>
+    <t>SARS-CoV-2</t>
+  </si>
+  <si>
+    <t>ILI</t>
+  </si>
+  <si>
+    <t>SARI</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>Hoja Global Resumen</t>
+  </si>
+  <si>
+    <t>Global semana epidemiologica</t>
+  </si>
+  <si>
+    <t>Hoja virus VRS</t>
+  </si>
+  <si>
+    <t>VRS</t>
+  </si>
+  <si>
+    <t>Hoja virus Ad</t>
+  </si>
+  <si>
+    <t>Hoja virus Parainfluenza</t>
+  </si>
+  <si>
+    <t>Parainfluenza</t>
+  </si>
+  <si>
+    <t>Hoja virus Inf A</t>
+  </si>
+  <si>
+    <t>Hoja virus Inf B</t>
+  </si>
+  <si>
+    <t>Hoja virus Metapnemovirus</t>
+  </si>
+  <si>
+    <t>Metapnemovirus</t>
+  </si>
+  <si>
+    <t>Hoja virus SARS-CoV-2</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Dominica</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -136,6 +195,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -441,49 +511,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -594,19 +621,6 @@
         <color indexed="64"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -836,11 +850,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -892,24 +957,12 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -934,34 +987,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -985,7 +1011,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -994,49 +1020,75 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1048,80 +1100,47 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="42" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="46" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1131,20 +1150,141 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="52" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="52" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="52" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1446,241 +1586,293 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:Q11"/>
+  <dimension ref="A2:S11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42.85546875" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="9" width="9.7109375" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" customWidth="1"/>
-    <col min="12" max="256" width="11.42578125" customWidth="1"/>
+    <col min="4" max="10" width="9.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" customWidth="1"/>
+    <col min="13" max="257" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="64" t="s">
+    <row r="2" spans="1:19" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="121" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="64"/>
-    </row>
-    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="65" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="65" t="s">
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="121"/>
+      <c r="L2" s="121"/>
+      <c r="M2" s="121"/>
+      <c r="N2" s="121"/>
+      <c r="O2" s="121"/>
+      <c r="P2" s="121"/>
+      <c r="Q2" s="121"/>
+      <c r="R2" s="121"/>
+      <c r="S2" s="121"/>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="49" t="str">
+        <f>Parameters!$B$11 &amp; ": " &amp; Parameters!$C$11</f>
+        <v>Country: Dominica</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="49" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:17" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="122" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="123"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="124"/>
+      <c r="F6" s="124"/>
+      <c r="G6" s="124"/>
+      <c r="H6" s="124"/>
+      <c r="I6" s="124"/>
+      <c r="J6" s="125"/>
+      <c r="K6" s="126" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" s="127"/>
+      <c r="M6" s="128"/>
+      <c r="N6" s="128"/>
+      <c r="O6" s="128"/>
+      <c r="P6" s="128"/>
+      <c r="Q6" s="128"/>
+      <c r="R6" s="128"/>
+      <c r="S6" s="129"/>
+    </row>
+    <row r="7" spans="1:19" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="104" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" s="10" t="s">
+      <c r="E7" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="105" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="105" t="s">
         <v>3</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="105" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="106" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="L7" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="19" t="s">
+      <c r="M7" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="M7" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="N7" s="20" t="s">
+      <c r="N7" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="O7" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="O7" s="20" t="s">
+      <c r="P7" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="P7" s="20" t="s">
+      <c r="Q7" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="Q7" s="21" t="s">
+      <c r="R7" s="34" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="31"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="40"/>
-      <c r="N8" s="40"/>
-      <c r="O8" s="40"/>
-      <c r="P8" s="40"/>
-      <c r="Q8" s="41"/>
-    </row>
-    <row r="9" spans="1:17" s="1" customFormat="1" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="66" t="s">
+      <c r="S7" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="27"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="100"/>
+      <c r="D8" s="107"/>
+      <c r="E8" s="108"/>
+      <c r="F8" s="108"/>
+      <c r="G8" s="108"/>
+      <c r="H8" s="108"/>
+      <c r="I8" s="108"/>
+      <c r="J8" s="109"/>
+      <c r="K8" s="102"/>
+      <c r="L8" s="94"/>
+      <c r="M8" s="96"/>
+      <c r="N8" s="97"/>
+      <c r="O8" s="97"/>
+      <c r="P8" s="97"/>
+      <c r="Q8" s="97"/>
+      <c r="R8" s="97"/>
+      <c r="S8" s="98"/>
+    </row>
+    <row r="9" spans="1:19" s="1" customFormat="1" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="50" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="6"/>
+      <c r="D9" s="103"/>
+      <c r="E9" s="103"/>
+      <c r="F9" s="103"/>
+      <c r="G9" s="103"/>
+      <c r="H9" s="103"/>
+      <c r="I9" s="103"/>
+      <c r="J9" s="103"/>
+      <c r="K9" s="19"/>
       <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-    </row>
-    <row r="10" spans="1:17" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="50"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="54"/>
-      <c r="L10" s="55"/>
-      <c r="M10" s="55"/>
-      <c r="N10" s="55"/>
-      <c r="O10" s="55"/>
-      <c r="P10" s="55"/>
-      <c r="Q10" s="56"/>
-    </row>
-    <row r="11" spans="1:17" s="2" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="49" t="s">
+      <c r="M9" s="95"/>
+      <c r="N9" s="95"/>
+      <c r="O9" s="95"/>
+      <c r="P9" s="95"/>
+      <c r="Q9" s="95"/>
+      <c r="R9" s="95"/>
+      <c r="S9" s="113"/>
+    </row>
+    <row r="10" spans="1:19" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="22"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="110"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="112"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="41"/>
+      <c r="P10" s="41"/>
+      <c r="Q10" s="41"/>
+      <c r="R10" s="111"/>
+      <c r="S10" s="42"/>
+    </row>
+    <row r="11" spans="1:19" s="2" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="36" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="15">
         <f>SUM(B8:B10)</f>
         <v>0</v>
       </c>
-      <c r="C11" s="23">
-        <f t="shared" ref="C11:I11" si="0">SUM(C8:C10)</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E11" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H11" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I11" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="57">
-        <f>SUM(J8:J10)</f>
-        <v>0</v>
-      </c>
-      <c r="K11" s="57">
+      <c r="C11" s="20">
+        <f t="shared" ref="C11:J11" si="0">SUM(C8:C10)</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="107">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="108">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="108">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="108">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="108">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="108">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="109">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K11" s="48">
         <f>SUM(K8:K10)</f>
         <v>0</v>
       </c>
-      <c r="L11" s="62">
-        <f t="shared" ref="L11:Q11" si="1">SUM(L8:L10)</f>
-        <v>0</v>
-      </c>
-      <c r="M11" s="62">
+      <c r="L11" s="43">
+        <f>SUM(L8:L10)</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="44">
+        <f t="shared" ref="M11:S11" si="1">SUM(M8:M10)</f>
+        <v>0</v>
+      </c>
+      <c r="N11" s="45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N11" s="62">
+      <c r="O11" s="45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O11" s="62">
+      <c r="P11" s="45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P11" s="62">
+      <c r="Q11" s="45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q11" s="63">
+      <c r="R11" s="45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="S11" s="46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:Q2"/>
+  <mergeCells count="3">
+    <mergeCell ref="B6:J6"/>
+    <mergeCell ref="K6:S6"/>
+    <mergeCell ref="A2:S2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="360" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -1689,7 +1881,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:W11"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1704,39 +1899,73 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:23" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="121" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="64"/>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="121"/>
+      <c r="L2" s="121"/>
+      <c r="M2" s="121"/>
+      <c r="N2" s="121"/>
+      <c r="O2" s="121"/>
+      <c r="P2" s="121"/>
+      <c r="Q2" s="121"/>
+      <c r="R2" s="121"/>
+      <c r="S2" s="121"/>
+      <c r="T2" s="121"/>
+      <c r="U2" s="121"/>
+      <c r="V2" s="121"/>
+      <c r="W2" s="121"/>
     </row>
     <row r="3" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="49" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="49" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:23" s="43" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="97" t="s">
+    <row r="5" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="130" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="131"/>
+      <c r="D6" s="131"/>
+      <c r="E6" s="131"/>
+      <c r="F6" s="131"/>
+      <c r="G6" s="131"/>
+      <c r="H6" s="131"/>
+      <c r="I6" s="131"/>
+      <c r="J6" s="131"/>
+      <c r="K6" s="131"/>
+      <c r="L6" s="132"/>
+      <c r="M6" s="133" t="s">
+        <v>26</v>
+      </c>
+      <c r="N6" s="134"/>
+      <c r="O6" s="134"/>
+      <c r="P6" s="134"/>
+      <c r="Q6" s="134"/>
+      <c r="R6" s="134"/>
+      <c r="S6" s="134"/>
+      <c r="T6" s="134"/>
+      <c r="U6" s="134"/>
+      <c r="V6" s="134"/>
+      <c r="W6" s="135"/>
+    </row>
+    <row r="7" spans="1:23" s="30" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="81" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -1760,13 +1989,13 @@
       <c r="H7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="42" t="s">
+      <c r="I7" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="42" t="s">
+      <c r="J7" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="K7" s="42" t="s">
+      <c r="K7" s="29" t="s">
         <v>20</v>
       </c>
       <c r="L7" s="11" t="s">
@@ -1778,116 +2007,116 @@
       <c r="N7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="46" t="s">
+      <c r="O7" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="P7" s="47" t="s">
+      <c r="P7" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="Q7" s="47" t="s">
+      <c r="Q7" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="R7" s="47" t="s">
+      <c r="R7" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="S7" s="47" t="s">
+      <c r="S7" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="T7" s="47" t="s">
+      <c r="T7" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="U7" s="47" t="s">
+      <c r="U7" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="47" t="s">
+      <c r="V7" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="W7" s="48" t="s">
+      <c r="W7" s="35" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="98"/>
-      <c r="B8" s="67"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="70"/>
-      <c r="I8" s="71"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="72"/>
-      <c r="M8" s="73"/>
-      <c r="N8" s="74"/>
-      <c r="O8" s="75"/>
-      <c r="P8" s="76"/>
-      <c r="Q8" s="76"/>
-      <c r="R8" s="76"/>
-      <c r="S8" s="76"/>
-      <c r="T8" s="76"/>
-      <c r="U8" s="76"/>
-      <c r="V8" s="77"/>
-      <c r="W8" s="78"/>
+      <c r="A8" s="82"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="56"/>
+      <c r="M8" s="57"/>
+      <c r="N8" s="58"/>
+      <c r="O8" s="59"/>
+      <c r="P8" s="60"/>
+      <c r="Q8" s="60"/>
+      <c r="R8" s="60"/>
+      <c r="S8" s="60"/>
+      <c r="T8" s="60"/>
+      <c r="U8" s="60"/>
+      <c r="V8" s="61"/>
+      <c r="W8" s="62"/>
     </row>
     <row r="9" spans="1:23" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="99" t="s">
+      <c r="A9" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="102"/>
-      <c r="C9" s="90"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="90"/>
-      <c r="G9" s="90"/>
-      <c r="H9" s="90"/>
-      <c r="I9" s="90"/>
-      <c r="J9" s="90"/>
-      <c r="K9" s="90"/>
-      <c r="L9" s="90"/>
-      <c r="M9" s="91"/>
-      <c r="N9" s="91"/>
-      <c r="O9" s="91"/>
-      <c r="P9" s="91"/>
-      <c r="Q9" s="91"/>
-      <c r="R9" s="91"/>
-      <c r="S9" s="91"/>
-      <c r="T9" s="91"/>
-      <c r="U9" s="91"/>
-      <c r="V9" s="91"/>
-      <c r="W9" s="91"/>
+      <c r="B9" s="86"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="74"/>
+      <c r="K9" s="74"/>
+      <c r="L9" s="74"/>
+      <c r="M9" s="75"/>
+      <c r="N9" s="75"/>
+      <c r="O9" s="75"/>
+      <c r="P9" s="75"/>
+      <c r="Q9" s="75"/>
+      <c r="R9" s="75"/>
+      <c r="S9" s="75"/>
+      <c r="T9" s="75"/>
+      <c r="U9" s="75"/>
+      <c r="V9" s="75"/>
+      <c r="W9" s="75"/>
     </row>
     <row r="10" spans="1:23" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="100"/>
-      <c r="B10" s="79"/>
-      <c r="C10" s="80"/>
-      <c r="D10" s="81"/>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="82"/>
-      <c r="I10" s="83"/>
-      <c r="J10" s="83"/>
-      <c r="K10" s="83"/>
-      <c r="L10" s="83"/>
-      <c r="M10" s="104"/>
-      <c r="N10" s="105"/>
-      <c r="O10" s="106"/>
-      <c r="P10" s="107"/>
-      <c r="Q10" s="107"/>
-      <c r="R10" s="107"/>
-      <c r="S10" s="107"/>
-      <c r="T10" s="107"/>
-      <c r="U10" s="107"/>
-      <c r="V10" s="107"/>
-      <c r="W10" s="108"/>
+      <c r="A10" s="84"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="67"/>
+      <c r="J10" s="67"/>
+      <c r="K10" s="67"/>
+      <c r="L10" s="67"/>
+      <c r="M10" s="88"/>
+      <c r="N10" s="89"/>
+      <c r="O10" s="90"/>
+      <c r="P10" s="91"/>
+      <c r="Q10" s="91"/>
+      <c r="R10" s="91"/>
+      <c r="S10" s="91"/>
+      <c r="T10" s="91"/>
+      <c r="U10" s="91"/>
+      <c r="V10" s="91"/>
+      <c r="W10" s="92"/>
     </row>
     <row r="11" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="101" t="s">
+      <c r="A11" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="61">
+      <c r="B11" s="47">
         <f t="shared" ref="B11:W11" si="0">SUM(B8:B10)</f>
         <v>0</v>
       </c>
@@ -1931,54 +2160,56 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M11" s="57">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N11" s="57">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O11" s="58">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P11" s="59">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="59">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R11" s="59">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="S11" s="59">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T11" s="59">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="U11" s="59">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V11" s="59">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W11" s="60">
+      <c r="M11" s="43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P11" s="45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R11" s="45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S11" s="45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T11" s="45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U11" s="45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V11" s="45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W11" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:Q2"/>
+  <mergeCells count="3">
+    <mergeCell ref="B6:L6"/>
+    <mergeCell ref="M6:W6"/>
+    <mergeCell ref="A2:W2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1989,7 +2220,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:W11"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2004,42 +2238,76 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:23" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="121" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="64"/>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="121"/>
+      <c r="L2" s="121"/>
+      <c r="M2" s="121"/>
+      <c r="N2" s="121"/>
+      <c r="O2" s="121"/>
+      <c r="P2" s="121"/>
+      <c r="Q2" s="121"/>
+      <c r="R2" s="121"/>
+      <c r="S2" s="121"/>
+      <c r="T2" s="121"/>
+      <c r="U2" s="121"/>
+      <c r="V2" s="121"/>
+      <c r="W2" s="121"/>
     </row>
     <row r="3" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="49" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="49" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:23" s="44" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="103" t="s">
+    <row r="5" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="130" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="131"/>
+      <c r="D6" s="131"/>
+      <c r="E6" s="131"/>
+      <c r="F6" s="131"/>
+      <c r="G6" s="131"/>
+      <c r="H6" s="131"/>
+      <c r="I6" s="131"/>
+      <c r="J6" s="131"/>
+      <c r="K6" s="131"/>
+      <c r="L6" s="132"/>
+      <c r="M6" s="133" t="s">
+        <v>26</v>
+      </c>
+      <c r="N6" s="134"/>
+      <c r="O6" s="134"/>
+      <c r="P6" s="134"/>
+      <c r="Q6" s="134"/>
+      <c r="R6" s="134"/>
+      <c r="S6" s="134"/>
+      <c r="T6" s="134"/>
+      <c r="U6" s="134"/>
+      <c r="V6" s="134"/>
+      <c r="W6" s="135"/>
+    </row>
+    <row r="7" spans="1:23" s="31" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="92" t="s">
+      <c r="B7" s="76" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="8" t="s">
@@ -2060,13 +2328,13 @@
       <c r="H7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="42" t="s">
+      <c r="I7" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="42" t="s">
+      <c r="J7" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="K7" s="42" t="s">
+      <c r="K7" s="29" t="s">
         <v>20</v>
       </c>
       <c r="L7" s="11" t="s">
@@ -2078,116 +2346,116 @@
       <c r="N7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="46" t="s">
+      <c r="O7" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="P7" s="47" t="s">
+      <c r="P7" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="Q7" s="47" t="s">
+      <c r="Q7" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="R7" s="47" t="s">
+      <c r="R7" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="S7" s="47" t="s">
+      <c r="S7" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="T7" s="47" t="s">
+      <c r="T7" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="U7" s="47" t="s">
+      <c r="U7" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="47" t="s">
+      <c r="V7" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="W7" s="48" t="s">
+      <c r="W7" s="35" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="98"/>
-      <c r="B8" s="93"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="70"/>
-      <c r="I8" s="70"/>
-      <c r="J8" s="70"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="72"/>
-      <c r="M8" s="73"/>
-      <c r="N8" s="74"/>
-      <c r="O8" s="75"/>
-      <c r="P8" s="76"/>
-      <c r="Q8" s="76"/>
-      <c r="R8" s="76"/>
-      <c r="S8" s="76"/>
-      <c r="T8" s="76"/>
-      <c r="U8" s="76"/>
-      <c r="V8" s="77"/>
-      <c r="W8" s="78"/>
+      <c r="A8" s="82"/>
+      <c r="B8" s="77"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="56"/>
+      <c r="M8" s="57"/>
+      <c r="N8" s="58"/>
+      <c r="O8" s="59"/>
+      <c r="P8" s="60"/>
+      <c r="Q8" s="60"/>
+      <c r="R8" s="60"/>
+      <c r="S8" s="60"/>
+      <c r="T8" s="60"/>
+      <c r="U8" s="60"/>
+      <c r="V8" s="61"/>
+      <c r="W8" s="62"/>
     </row>
     <row r="9" spans="1:23" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="99" t="s">
+      <c r="A9" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="90"/>
-      <c r="C9" s="90"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="90"/>
-      <c r="G9" s="90"/>
-      <c r="H9" s="90"/>
-      <c r="I9" s="90"/>
-      <c r="J9" s="90"/>
-      <c r="K9" s="90"/>
-      <c r="L9" s="90"/>
-      <c r="M9" s="91"/>
-      <c r="N9" s="91"/>
-      <c r="O9" s="91"/>
-      <c r="P9" s="91"/>
-      <c r="Q9" s="91"/>
-      <c r="R9" s="91"/>
-      <c r="S9" s="91"/>
-      <c r="T9" s="91"/>
-      <c r="U9" s="91"/>
-      <c r="V9" s="91"/>
-      <c r="W9" s="91"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="74"/>
+      <c r="K9" s="74"/>
+      <c r="L9" s="74"/>
+      <c r="M9" s="75"/>
+      <c r="N9" s="75"/>
+      <c r="O9" s="75"/>
+      <c r="P9" s="75"/>
+      <c r="Q9" s="75"/>
+      <c r="R9" s="75"/>
+      <c r="S9" s="75"/>
+      <c r="T9" s="75"/>
+      <c r="U9" s="75"/>
+      <c r="V9" s="75"/>
+      <c r="W9" s="75"/>
     </row>
     <row r="10" spans="1:23" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="100"/>
-      <c r="B10" s="95"/>
-      <c r="C10" s="80"/>
-      <c r="D10" s="81"/>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="82"/>
-      <c r="I10" s="82"/>
-      <c r="J10" s="82"/>
-      <c r="K10" s="83"/>
-      <c r="L10" s="84"/>
-      <c r="M10" s="85"/>
-      <c r="N10" s="86"/>
-      <c r="O10" s="87"/>
-      <c r="P10" s="88"/>
-      <c r="Q10" s="88"/>
-      <c r="R10" s="88"/>
-      <c r="S10" s="88"/>
-      <c r="T10" s="88"/>
-      <c r="U10" s="88"/>
-      <c r="V10" s="88"/>
-      <c r="W10" s="89"/>
+      <c r="A10" s="84"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="66"/>
+      <c r="J10" s="66"/>
+      <c r="K10" s="67"/>
+      <c r="L10" s="68"/>
+      <c r="M10" s="69"/>
+      <c r="N10" s="70"/>
+      <c r="O10" s="71"/>
+      <c r="P10" s="72"/>
+      <c r="Q10" s="72"/>
+      <c r="R10" s="72"/>
+      <c r="S10" s="72"/>
+      <c r="T10" s="72"/>
+      <c r="U10" s="72"/>
+      <c r="V10" s="72"/>
+      <c r="W10" s="73"/>
     </row>
     <row r="11" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="101" t="s">
+      <c r="A11" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="96">
+      <c r="B11" s="80">
         <f t="shared" ref="B11:W11" si="0">SUM(B8:B10)</f>
         <v>0</v>
       </c>
@@ -2231,15 +2499,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M11" s="45">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N11" s="45">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O11" s="51">
+      <c r="M11" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="38">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2271,14 +2539,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W11" s="52">
+      <c r="W11" s="39">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:Q2"/>
+  <mergeCells count="3">
+    <mergeCell ref="B6:L6"/>
+    <mergeCell ref="M6:W6"/>
+    <mergeCell ref="A2:W2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2289,7 +2559,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:W11"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2304,42 +2577,76 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:23" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="121" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="64"/>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="121"/>
+      <c r="L2" s="121"/>
+      <c r="M2" s="121"/>
+      <c r="N2" s="121"/>
+      <c r="O2" s="121"/>
+      <c r="P2" s="121"/>
+      <c r="Q2" s="121"/>
+      <c r="R2" s="121"/>
+      <c r="S2" s="121"/>
+      <c r="T2" s="121"/>
+      <c r="U2" s="121"/>
+      <c r="V2" s="121"/>
+      <c r="W2" s="121"/>
     </row>
     <row r="3" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="49" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="49" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="130" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="131"/>
+      <c r="D6" s="131"/>
+      <c r="E6" s="131"/>
+      <c r="F6" s="131"/>
+      <c r="G6" s="131"/>
+      <c r="H6" s="131"/>
+      <c r="I6" s="131"/>
+      <c r="J6" s="131"/>
+      <c r="K6" s="131"/>
+      <c r="L6" s="132"/>
+      <c r="M6" s="133" t="s">
+        <v>26</v>
+      </c>
+      <c r="N6" s="134"/>
+      <c r="O6" s="134"/>
+      <c r="P6" s="134"/>
+      <c r="Q6" s="134"/>
+      <c r="R6" s="134"/>
+      <c r="S6" s="134"/>
+      <c r="T6" s="134"/>
+      <c r="U6" s="134"/>
+      <c r="V6" s="134"/>
+      <c r="W6" s="135"/>
+    </row>
     <row r="7" spans="1:23" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="103" t="s">
+      <c r="A7" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="92" t="s">
+      <c r="B7" s="76" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="8" t="s">
@@ -2360,13 +2667,13 @@
       <c r="H7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="42" t="s">
+      <c r="I7" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="42" t="s">
+      <c r="J7" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="K7" s="42" t="s">
+      <c r="K7" s="29" t="s">
         <v>20</v>
       </c>
       <c r="L7" s="11" t="s">
@@ -2378,116 +2685,116 @@
       <c r="N7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="46" t="s">
+      <c r="O7" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="P7" s="47" t="s">
+      <c r="P7" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="Q7" s="47" t="s">
+      <c r="Q7" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="R7" s="47" t="s">
+      <c r="R7" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="S7" s="47" t="s">
+      <c r="S7" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="T7" s="47" t="s">
+      <c r="T7" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="U7" s="47" t="s">
+      <c r="U7" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="47" t="s">
+      <c r="V7" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="W7" s="48" t="s">
+      <c r="W7" s="35" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="98"/>
-      <c r="B8" s="93"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="70"/>
-      <c r="I8" s="71"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="72"/>
-      <c r="M8" s="73"/>
-      <c r="N8" s="74"/>
-      <c r="O8" s="75"/>
-      <c r="P8" s="76"/>
-      <c r="Q8" s="76"/>
-      <c r="R8" s="76"/>
-      <c r="S8" s="76"/>
-      <c r="T8" s="76"/>
-      <c r="U8" s="76"/>
-      <c r="V8" s="77"/>
-      <c r="W8" s="78"/>
+      <c r="A8" s="82"/>
+      <c r="B8" s="77"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="56"/>
+      <c r="M8" s="57"/>
+      <c r="N8" s="58"/>
+      <c r="O8" s="59"/>
+      <c r="P8" s="60"/>
+      <c r="Q8" s="60"/>
+      <c r="R8" s="60"/>
+      <c r="S8" s="60"/>
+      <c r="T8" s="60"/>
+      <c r="U8" s="60"/>
+      <c r="V8" s="61"/>
+      <c r="W8" s="62"/>
     </row>
     <row r="9" spans="1:23" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="99" t="s">
+      <c r="A9" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="90"/>
-      <c r="C9" s="90"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="90"/>
-      <c r="G9" s="90"/>
-      <c r="H9" s="90"/>
-      <c r="I9" s="90"/>
-      <c r="J9" s="90"/>
-      <c r="K9" s="90"/>
-      <c r="L9" s="90"/>
-      <c r="M9" s="91"/>
-      <c r="N9" s="91"/>
-      <c r="O9" s="91"/>
-      <c r="P9" s="91"/>
-      <c r="Q9" s="91"/>
-      <c r="R9" s="91"/>
-      <c r="S9" s="91"/>
-      <c r="T9" s="91"/>
-      <c r="U9" s="91"/>
-      <c r="V9" s="91"/>
-      <c r="W9" s="91"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="74"/>
+      <c r="K9" s="74"/>
+      <c r="L9" s="74"/>
+      <c r="M9" s="75"/>
+      <c r="N9" s="75"/>
+      <c r="O9" s="75"/>
+      <c r="P9" s="75"/>
+      <c r="Q9" s="75"/>
+      <c r="R9" s="75"/>
+      <c r="S9" s="75"/>
+      <c r="T9" s="75"/>
+      <c r="U9" s="75"/>
+      <c r="V9" s="75"/>
+      <c r="W9" s="75"/>
     </row>
     <row r="10" spans="1:23" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="100"/>
-      <c r="B10" s="95"/>
-      <c r="C10" s="80"/>
-      <c r="D10" s="81"/>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="82"/>
-      <c r="I10" s="83"/>
-      <c r="J10" s="83"/>
-      <c r="K10" s="83"/>
-      <c r="L10" s="84"/>
-      <c r="M10" s="85"/>
-      <c r="N10" s="86"/>
-      <c r="O10" s="87"/>
-      <c r="P10" s="88"/>
-      <c r="Q10" s="88"/>
-      <c r="R10" s="88"/>
-      <c r="S10" s="88"/>
-      <c r="T10" s="88"/>
-      <c r="U10" s="88"/>
-      <c r="V10" s="88"/>
-      <c r="W10" s="89"/>
+      <c r="A10" s="84"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="67"/>
+      <c r="J10" s="67"/>
+      <c r="K10" s="67"/>
+      <c r="L10" s="68"/>
+      <c r="M10" s="69"/>
+      <c r="N10" s="70"/>
+      <c r="O10" s="71"/>
+      <c r="P10" s="72"/>
+      <c r="Q10" s="72"/>
+      <c r="R10" s="72"/>
+      <c r="S10" s="72"/>
+      <c r="T10" s="72"/>
+      <c r="U10" s="72"/>
+      <c r="V10" s="72"/>
+      <c r="W10" s="73"/>
     </row>
     <row r="11" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="101" t="s">
+      <c r="A11" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="96">
+      <c r="B11" s="80">
         <f t="shared" ref="B11:W11" si="0">SUM(B8:B10)</f>
         <v>0</v>
       </c>
@@ -2531,15 +2838,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M11" s="45">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N11" s="45">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O11" s="51">
+      <c r="M11" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="38">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2571,14 +2878,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W11" s="52">
+      <c r="W11" s="39">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:Q2"/>
+  <mergeCells count="3">
+    <mergeCell ref="B6:L6"/>
+    <mergeCell ref="M6:W6"/>
+    <mergeCell ref="A2:W2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2588,7 +2897,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:W11"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2603,42 +2915,76 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:23" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="121" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="64"/>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="121"/>
+      <c r="L2" s="121"/>
+      <c r="M2" s="121"/>
+      <c r="N2" s="121"/>
+      <c r="O2" s="121"/>
+      <c r="P2" s="121"/>
+      <c r="Q2" s="121"/>
+      <c r="R2" s="121"/>
+      <c r="S2" s="121"/>
+      <c r="T2" s="121"/>
+      <c r="U2" s="121"/>
+      <c r="V2" s="121"/>
+      <c r="W2" s="121"/>
     </row>
     <row r="3" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="49" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="49" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="130" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="131"/>
+      <c r="D6" s="131"/>
+      <c r="E6" s="131"/>
+      <c r="F6" s="131"/>
+      <c r="G6" s="131"/>
+      <c r="H6" s="131"/>
+      <c r="I6" s="131"/>
+      <c r="J6" s="131"/>
+      <c r="K6" s="131"/>
+      <c r="L6" s="132"/>
+      <c r="M6" s="133" t="s">
+        <v>26</v>
+      </c>
+      <c r="N6" s="134"/>
+      <c r="O6" s="134"/>
+      <c r="P6" s="134"/>
+      <c r="Q6" s="134"/>
+      <c r="R6" s="134"/>
+      <c r="S6" s="134"/>
+      <c r="T6" s="134"/>
+      <c r="U6" s="134"/>
+      <c r="V6" s="134"/>
+      <c r="W6" s="135"/>
+    </row>
     <row r="7" spans="1:23" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="103" t="s">
+      <c r="A7" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="92" t="s">
+      <c r="B7" s="76" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="8" t="s">
@@ -2659,13 +3005,13 @@
       <c r="H7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="42" t="s">
+      <c r="I7" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="42" t="s">
+      <c r="J7" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="K7" s="42" t="s">
+      <c r="K7" s="29" t="s">
         <v>20</v>
       </c>
       <c r="L7" s="11" t="s">
@@ -2677,116 +3023,116 @@
       <c r="N7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="46" t="s">
+      <c r="O7" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="P7" s="47" t="s">
+      <c r="P7" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="Q7" s="47" t="s">
+      <c r="Q7" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="R7" s="47" t="s">
+      <c r="R7" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="S7" s="47" t="s">
+      <c r="S7" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="T7" s="47" t="s">
+      <c r="T7" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="U7" s="47" t="s">
+      <c r="U7" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="47" t="s">
+      <c r="V7" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="W7" s="48" t="s">
+      <c r="W7" s="35" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="98"/>
-      <c r="B8" s="93"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="70"/>
-      <c r="I8" s="71"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="72"/>
-      <c r="M8" s="73"/>
-      <c r="N8" s="74"/>
-      <c r="O8" s="75"/>
-      <c r="P8" s="76"/>
-      <c r="Q8" s="76"/>
-      <c r="R8" s="76"/>
-      <c r="S8" s="76"/>
-      <c r="T8" s="76"/>
-      <c r="U8" s="76"/>
-      <c r="V8" s="77"/>
-      <c r="W8" s="78"/>
+      <c r="A8" s="82"/>
+      <c r="B8" s="77"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="56"/>
+      <c r="M8" s="57"/>
+      <c r="N8" s="58"/>
+      <c r="O8" s="59"/>
+      <c r="P8" s="60"/>
+      <c r="Q8" s="60"/>
+      <c r="R8" s="60"/>
+      <c r="S8" s="60"/>
+      <c r="T8" s="60"/>
+      <c r="U8" s="60"/>
+      <c r="V8" s="61"/>
+      <c r="W8" s="62"/>
     </row>
     <row r="9" spans="1:23" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="99" t="s">
+      <c r="A9" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="90"/>
-      <c r="C9" s="90"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="90"/>
-      <c r="G9" s="90"/>
-      <c r="H9" s="90"/>
-      <c r="I9" s="90"/>
-      <c r="J9" s="90"/>
-      <c r="K9" s="90"/>
-      <c r="L9" s="90"/>
-      <c r="M9" s="91"/>
-      <c r="N9" s="91"/>
-      <c r="O9" s="91"/>
-      <c r="P9" s="91"/>
-      <c r="Q9" s="91"/>
-      <c r="R9" s="91"/>
-      <c r="S9" s="91"/>
-      <c r="T9" s="91"/>
-      <c r="U9" s="91"/>
-      <c r="V9" s="91"/>
-      <c r="W9" s="91"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="74"/>
+      <c r="K9" s="74"/>
+      <c r="L9" s="74"/>
+      <c r="M9" s="75"/>
+      <c r="N9" s="75"/>
+      <c r="O9" s="75"/>
+      <c r="P9" s="75"/>
+      <c r="Q9" s="75"/>
+      <c r="R9" s="75"/>
+      <c r="S9" s="75"/>
+      <c r="T9" s="75"/>
+      <c r="U9" s="75"/>
+      <c r="V9" s="75"/>
+      <c r="W9" s="75"/>
     </row>
     <row r="10" spans="1:23" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="100"/>
-      <c r="B10" s="95"/>
-      <c r="C10" s="80"/>
-      <c r="D10" s="81"/>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="82"/>
-      <c r="I10" s="83"/>
-      <c r="J10" s="83"/>
-      <c r="K10" s="83"/>
-      <c r="L10" s="84"/>
-      <c r="M10" s="85"/>
-      <c r="N10" s="86"/>
-      <c r="O10" s="87"/>
-      <c r="P10" s="88"/>
-      <c r="Q10" s="88"/>
-      <c r="R10" s="88"/>
-      <c r="S10" s="88"/>
-      <c r="T10" s="88"/>
-      <c r="U10" s="88"/>
-      <c r="V10" s="88"/>
-      <c r="W10" s="89"/>
+      <c r="A10" s="84"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="67"/>
+      <c r="J10" s="67"/>
+      <c r="K10" s="67"/>
+      <c r="L10" s="68"/>
+      <c r="M10" s="69"/>
+      <c r="N10" s="70"/>
+      <c r="O10" s="71"/>
+      <c r="P10" s="72"/>
+      <c r="Q10" s="72"/>
+      <c r="R10" s="72"/>
+      <c r="S10" s="72"/>
+      <c r="T10" s="72"/>
+      <c r="U10" s="72"/>
+      <c r="V10" s="72"/>
+      <c r="W10" s="73"/>
     </row>
     <row r="11" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="101" t="s">
+      <c r="A11" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="96">
+      <c r="B11" s="80">
         <f t="shared" ref="B11:W11" si="0">SUM(B8:B10)</f>
         <v>0</v>
       </c>
@@ -2830,15 +3176,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M11" s="45">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N11" s="45">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O11" s="51">
+      <c r="M11" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="38">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2870,14 +3216,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W11" s="52">
+      <c r="W11" s="39">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:Q2"/>
+  <mergeCells count="3">
+    <mergeCell ref="B6:L6"/>
+    <mergeCell ref="M6:W6"/>
+    <mergeCell ref="A2:W2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2887,7 +3235,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:W11"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2902,42 +3253,76 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:23" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="121" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="64"/>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="121"/>
+      <c r="L2" s="121"/>
+      <c r="M2" s="121"/>
+      <c r="N2" s="121"/>
+      <c r="O2" s="121"/>
+      <c r="P2" s="121"/>
+      <c r="Q2" s="121"/>
+      <c r="R2" s="121"/>
+      <c r="S2" s="121"/>
+      <c r="T2" s="121"/>
+      <c r="U2" s="121"/>
+      <c r="V2" s="121"/>
+      <c r="W2" s="121"/>
     </row>
     <row r="3" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="49" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="49" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="130" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="131"/>
+      <c r="D6" s="131"/>
+      <c r="E6" s="131"/>
+      <c r="F6" s="131"/>
+      <c r="G6" s="131"/>
+      <c r="H6" s="131"/>
+      <c r="I6" s="131"/>
+      <c r="J6" s="131"/>
+      <c r="K6" s="131"/>
+      <c r="L6" s="132"/>
+      <c r="M6" s="133" t="s">
+        <v>26</v>
+      </c>
+      <c r="N6" s="134"/>
+      <c r="O6" s="134"/>
+      <c r="P6" s="134"/>
+      <c r="Q6" s="134"/>
+      <c r="R6" s="134"/>
+      <c r="S6" s="134"/>
+      <c r="T6" s="134"/>
+      <c r="U6" s="134"/>
+      <c r="V6" s="134"/>
+      <c r="W6" s="135"/>
+    </row>
     <row r="7" spans="1:23" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="103" t="s">
+      <c r="A7" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="92" t="s">
+      <c r="B7" s="76" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="8" t="s">
@@ -2958,13 +3343,13 @@
       <c r="H7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="42" t="s">
+      <c r="I7" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="42" t="s">
+      <c r="J7" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="K7" s="42" t="s">
+      <c r="K7" s="29" t="s">
         <v>20</v>
       </c>
       <c r="L7" s="11" t="s">
@@ -2976,116 +3361,116 @@
       <c r="N7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="46" t="s">
+      <c r="O7" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="P7" s="47" t="s">
+      <c r="P7" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="Q7" s="47" t="s">
+      <c r="Q7" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="R7" s="47" t="s">
+      <c r="R7" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="S7" s="47" t="s">
+      <c r="S7" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="T7" s="47" t="s">
+      <c r="T7" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="U7" s="47" t="s">
+      <c r="U7" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="47" t="s">
+      <c r="V7" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="W7" s="48" t="s">
+      <c r="W7" s="35" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="98"/>
-      <c r="B8" s="93"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="70"/>
-      <c r="I8" s="70"/>
-      <c r="J8" s="70"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="72"/>
-      <c r="M8" s="73"/>
-      <c r="N8" s="74"/>
-      <c r="O8" s="75"/>
-      <c r="P8" s="76"/>
-      <c r="Q8" s="76"/>
-      <c r="R8" s="76"/>
-      <c r="S8" s="76"/>
-      <c r="T8" s="76"/>
-      <c r="U8" s="76"/>
-      <c r="V8" s="77"/>
-      <c r="W8" s="78"/>
+      <c r="A8" s="82"/>
+      <c r="B8" s="77"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="56"/>
+      <c r="M8" s="57"/>
+      <c r="N8" s="58"/>
+      <c r="O8" s="59"/>
+      <c r="P8" s="60"/>
+      <c r="Q8" s="60"/>
+      <c r="R8" s="60"/>
+      <c r="S8" s="60"/>
+      <c r="T8" s="60"/>
+      <c r="U8" s="60"/>
+      <c r="V8" s="61"/>
+      <c r="W8" s="62"/>
     </row>
     <row r="9" spans="1:23" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="99" t="s">
+      <c r="A9" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="90"/>
-      <c r="C9" s="90"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="90"/>
-      <c r="G9" s="90"/>
-      <c r="H9" s="90"/>
-      <c r="I9" s="90"/>
-      <c r="J9" s="90"/>
-      <c r="K9" s="90"/>
-      <c r="L9" s="90"/>
-      <c r="M9" s="91"/>
-      <c r="N9" s="91"/>
-      <c r="O9" s="91"/>
-      <c r="P9" s="91"/>
-      <c r="Q9" s="91"/>
-      <c r="R9" s="91"/>
-      <c r="S9" s="91"/>
-      <c r="T9" s="91"/>
-      <c r="U9" s="91"/>
-      <c r="V9" s="91"/>
-      <c r="W9" s="91"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="74"/>
+      <c r="K9" s="74"/>
+      <c r="L9" s="74"/>
+      <c r="M9" s="75"/>
+      <c r="N9" s="75"/>
+      <c r="O9" s="75"/>
+      <c r="P9" s="75"/>
+      <c r="Q9" s="75"/>
+      <c r="R9" s="75"/>
+      <c r="S9" s="75"/>
+      <c r="T9" s="75"/>
+      <c r="U9" s="75"/>
+      <c r="V9" s="75"/>
+      <c r="W9" s="75"/>
     </row>
     <row r="10" spans="1:23" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="100"/>
-      <c r="B10" s="95"/>
-      <c r="C10" s="80"/>
-      <c r="D10" s="81"/>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="82"/>
-      <c r="I10" s="82"/>
-      <c r="J10" s="82"/>
-      <c r="K10" s="83"/>
-      <c r="L10" s="84"/>
-      <c r="M10" s="85"/>
-      <c r="N10" s="86"/>
-      <c r="O10" s="87"/>
-      <c r="P10" s="88"/>
-      <c r="Q10" s="88"/>
-      <c r="R10" s="88"/>
-      <c r="S10" s="88"/>
-      <c r="T10" s="88"/>
-      <c r="U10" s="88"/>
-      <c r="V10" s="88"/>
-      <c r="W10" s="89"/>
+      <c r="A10" s="84"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="66"/>
+      <c r="J10" s="66"/>
+      <c r="K10" s="67"/>
+      <c r="L10" s="68"/>
+      <c r="M10" s="69"/>
+      <c r="N10" s="70"/>
+      <c r="O10" s="71"/>
+      <c r="P10" s="72"/>
+      <c r="Q10" s="72"/>
+      <c r="R10" s="72"/>
+      <c r="S10" s="72"/>
+      <c r="T10" s="72"/>
+      <c r="U10" s="72"/>
+      <c r="V10" s="72"/>
+      <c r="W10" s="73"/>
     </row>
     <row r="11" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="101" t="s">
+      <c r="A11" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="96">
+      <c r="B11" s="80">
         <f t="shared" ref="B11:W11" si="0">SUM(B8:B10)</f>
         <v>0</v>
       </c>
@@ -3129,15 +3514,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M11" s="45">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N11" s="45">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O11" s="51">
+      <c r="M11" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="38">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3169,14 +3554,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W11" s="52">
+      <c r="W11" s="39">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:Q2"/>
+  <mergeCells count="3">
+    <mergeCell ref="B6:L6"/>
+    <mergeCell ref="M6:W6"/>
+    <mergeCell ref="A2:W2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3186,12 +3573,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W11"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="25" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="21" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" customWidth="1"/>
     <col min="4" max="12" width="9.28515625" customWidth="1"/>
     <col min="13" max="13" width="15.7109375" customWidth="1"/>
@@ -3204,44 +3594,78 @@
       <c r="B1"/>
     </row>
     <row r="2" spans="1:23" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="121" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="64"/>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="121"/>
+      <c r="L2" s="121"/>
+      <c r="M2" s="121"/>
+      <c r="N2" s="121"/>
+      <c r="O2" s="121"/>
+      <c r="P2" s="121"/>
+      <c r="Q2" s="121"/>
+      <c r="R2" s="121"/>
+      <c r="S2" s="121"/>
+      <c r="T2" s="121"/>
+      <c r="U2" s="121"/>
+      <c r="V2" s="121"/>
+      <c r="W2" s="121"/>
     </row>
     <row r="3" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="49" t="s">
         <v>22</v>
       </c>
       <c r="B3"/>
     </row>
     <row r="4" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="49" t="s">
         <v>23</v>
       </c>
       <c r="B4"/>
     </row>
-    <row r="6" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="130" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="131"/>
+      <c r="D6" s="131"/>
+      <c r="E6" s="131"/>
+      <c r="F6" s="131"/>
+      <c r="G6" s="131"/>
+      <c r="H6" s="131"/>
+      <c r="I6" s="131"/>
+      <c r="J6" s="131"/>
+      <c r="K6" s="131"/>
+      <c r="L6" s="132"/>
+      <c r="M6" s="133" t="s">
+        <v>26</v>
+      </c>
+      <c r="N6" s="134"/>
+      <c r="O6" s="134"/>
+      <c r="P6" s="134"/>
+      <c r="Q6" s="134"/>
+      <c r="R6" s="134"/>
+      <c r="S6" s="134"/>
+      <c r="T6" s="134"/>
+      <c r="U6" s="134"/>
+      <c r="V6" s="134"/>
+      <c r="W6" s="135"/>
+    </row>
     <row r="7" spans="1:23" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="97" t="s">
+      <c r="A7" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="92" t="s">
+      <c r="B7" s="76" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="8" t="s">
@@ -3262,13 +3686,13 @@
       <c r="H7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="42" t="s">
+      <c r="I7" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="42" t="s">
+      <c r="J7" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="K7" s="42" t="s">
+      <c r="K7" s="29" t="s">
         <v>20</v>
       </c>
       <c r="L7" s="11" t="s">
@@ -3280,116 +3704,116 @@
       <c r="N7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="46" t="s">
+      <c r="O7" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="P7" s="47" t="s">
+      <c r="P7" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="Q7" s="47" t="s">
+      <c r="Q7" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="R7" s="47" t="s">
+      <c r="R7" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="S7" s="47" t="s">
+      <c r="S7" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="T7" s="47" t="s">
+      <c r="T7" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="U7" s="47" t="s">
+      <c r="U7" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="47" t="s">
+      <c r="V7" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="W7" s="48" t="s">
+      <c r="W7" s="35" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="98"/>
-      <c r="B8" s="93"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="70"/>
-      <c r="I8" s="71"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="72"/>
-      <c r="M8" s="73"/>
-      <c r="N8" s="74"/>
-      <c r="O8" s="75"/>
-      <c r="P8" s="76"/>
-      <c r="Q8" s="76"/>
-      <c r="R8" s="76"/>
-      <c r="S8" s="76"/>
-      <c r="T8" s="76"/>
-      <c r="U8" s="76"/>
-      <c r="V8" s="77"/>
-      <c r="W8" s="78"/>
+      <c r="A8" s="82"/>
+      <c r="B8" s="77"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="56"/>
+      <c r="M8" s="57"/>
+      <c r="N8" s="58"/>
+      <c r="O8" s="59"/>
+      <c r="P8" s="60"/>
+      <c r="Q8" s="60"/>
+      <c r="R8" s="60"/>
+      <c r="S8" s="60"/>
+      <c r="T8" s="60"/>
+      <c r="U8" s="60"/>
+      <c r="V8" s="61"/>
+      <c r="W8" s="62"/>
     </row>
     <row r="9" spans="1:23" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="99" t="s">
+      <c r="A9" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="94"/>
-      <c r="C9" s="90"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="90"/>
-      <c r="G9" s="90"/>
-      <c r="H9" s="90"/>
-      <c r="I9" s="90"/>
-      <c r="J9" s="90"/>
-      <c r="K9" s="90"/>
-      <c r="L9" s="90"/>
-      <c r="M9" s="91"/>
-      <c r="N9" s="91"/>
-      <c r="O9" s="91"/>
-      <c r="P9" s="91"/>
-      <c r="Q9" s="91"/>
-      <c r="R9" s="91"/>
-      <c r="S9" s="91"/>
-      <c r="T9" s="91"/>
-      <c r="U9" s="91"/>
-      <c r="V9" s="91"/>
-      <c r="W9" s="91"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="74"/>
+      <c r="K9" s="74"/>
+      <c r="L9" s="74"/>
+      <c r="M9" s="75"/>
+      <c r="N9" s="75"/>
+      <c r="O9" s="75"/>
+      <c r="P9" s="75"/>
+      <c r="Q9" s="75"/>
+      <c r="R9" s="75"/>
+      <c r="S9" s="75"/>
+      <c r="T9" s="75"/>
+      <c r="U9" s="75"/>
+      <c r="V9" s="75"/>
+      <c r="W9" s="75"/>
     </row>
     <row r="10" spans="1:23" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="100"/>
-      <c r="B10" s="95"/>
-      <c r="C10" s="80"/>
-      <c r="D10" s="81"/>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="82"/>
-      <c r="I10" s="83"/>
-      <c r="J10" s="83"/>
-      <c r="K10" s="83"/>
-      <c r="L10" s="84"/>
-      <c r="M10" s="85"/>
-      <c r="N10" s="86"/>
-      <c r="O10" s="87"/>
-      <c r="P10" s="88"/>
-      <c r="Q10" s="88"/>
-      <c r="R10" s="88"/>
-      <c r="S10" s="88"/>
-      <c r="T10" s="88"/>
-      <c r="U10" s="88"/>
-      <c r="V10" s="88"/>
-      <c r="W10" s="89"/>
+      <c r="A10" s="84"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="67"/>
+      <c r="J10" s="67"/>
+      <c r="K10" s="67"/>
+      <c r="L10" s="68"/>
+      <c r="M10" s="69"/>
+      <c r="N10" s="70"/>
+      <c r="O10" s="71"/>
+      <c r="P10" s="72"/>
+      <c r="Q10" s="72"/>
+      <c r="R10" s="72"/>
+      <c r="S10" s="72"/>
+      <c r="T10" s="72"/>
+      <c r="U10" s="72"/>
+      <c r="V10" s="72"/>
+      <c r="W10" s="73"/>
     </row>
     <row r="11" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="101" t="s">
+      <c r="A11" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="96">
+      <c r="B11" s="80">
         <f t="shared" ref="B11:W11" si="0">SUM(B8:B10)</f>
         <v>0</v>
       </c>
@@ -3433,15 +3857,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M11" s="45">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N11" s="45">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O11" s="51">
+      <c r="M11" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="38">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3473,15 +3897,464 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W11" s="52">
+      <c r="W11" s="39">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:Q2"/>
+  <mergeCells count="3">
+    <mergeCell ref="B6:L6"/>
+    <mergeCell ref="M6:W6"/>
+    <mergeCell ref="A2:W2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W11"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="42.7109375" style="114" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="119" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="114" customWidth="1"/>
+    <col min="4" max="12" width="9.28515625" style="114" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" style="114" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" style="114" customWidth="1"/>
+    <col min="15" max="23" width="9.28515625" style="114" customWidth="1"/>
+    <col min="24" max="256" width="11.42578125" style="114" customWidth="1"/>
+    <col min="257" max="16384" width="9.140625" style="114"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B1" s="114"/>
+    </row>
+    <row r="2" spans="1:23" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="136" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="136"/>
+      <c r="C2" s="136"/>
+      <c r="D2" s="136"/>
+      <c r="E2" s="136"/>
+      <c r="F2" s="136"/>
+      <c r="G2" s="136"/>
+      <c r="H2" s="136"/>
+      <c r="I2" s="136"/>
+      <c r="J2" s="136"/>
+      <c r="K2" s="136"/>
+      <c r="L2" s="136"/>
+      <c r="M2" s="136"/>
+      <c r="N2" s="136"/>
+      <c r="O2" s="136"/>
+      <c r="P2" s="136"/>
+      <c r="Q2" s="136"/>
+      <c r="R2" s="136"/>
+      <c r="S2" s="136"/>
+      <c r="T2" s="136"/>
+      <c r="U2" s="136"/>
+      <c r="V2" s="136"/>
+      <c r="W2" s="136"/>
+    </row>
+    <row r="3" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="115" t="str">
+        <f>Parameters!$B$11 &amp; ": " &amp; Parameters!$C$11</f>
+        <v>Country: Dominica</v>
+      </c>
+      <c r="B3" s="114"/>
+    </row>
+    <row r="4" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="115" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="114"/>
+    </row>
+    <row r="5" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="114"/>
+    </row>
+    <row r="6" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="130" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="131"/>
+      <c r="D6" s="131"/>
+      <c r="E6" s="131"/>
+      <c r="F6" s="131"/>
+      <c r="G6" s="131"/>
+      <c r="H6" s="131"/>
+      <c r="I6" s="131"/>
+      <c r="J6" s="131"/>
+      <c r="K6" s="131"/>
+      <c r="L6" s="132"/>
+      <c r="M6" s="133" t="s">
+        <v>26</v>
+      </c>
+      <c r="N6" s="134"/>
+      <c r="O6" s="134"/>
+      <c r="P6" s="134"/>
+      <c r="Q6" s="134"/>
+      <c r="R6" s="134"/>
+      <c r="S6" s="134"/>
+      <c r="T6" s="134"/>
+      <c r="U6" s="134"/>
+      <c r="V6" s="134"/>
+      <c r="W6" s="135"/>
+    </row>
+    <row r="7" spans="1:23" s="116" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O7" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="P7" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q7" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="R7" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="S7" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="T7" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="U7" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="V7" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="W7" s="35" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" s="117" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="82"/>
+      <c r="B8" s="77"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="56"/>
+      <c r="M8" s="57"/>
+      <c r="N8" s="58"/>
+      <c r="O8" s="59"/>
+      <c r="P8" s="60"/>
+      <c r="Q8" s="60"/>
+      <c r="R8" s="60"/>
+      <c r="S8" s="60"/>
+      <c r="T8" s="60"/>
+      <c r="U8" s="60"/>
+      <c r="V8" s="61"/>
+      <c r="W8" s="62"/>
+    </row>
+    <row r="9" spans="1:23" s="118" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="83" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="78"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="74"/>
+      <c r="K9" s="74"/>
+      <c r="L9" s="74"/>
+      <c r="M9" s="75"/>
+      <c r="N9" s="75"/>
+      <c r="O9" s="75"/>
+      <c r="P9" s="75"/>
+      <c r="Q9" s="75"/>
+      <c r="R9" s="75"/>
+      <c r="S9" s="75"/>
+      <c r="T9" s="75"/>
+      <c r="U9" s="75"/>
+      <c r="V9" s="75"/>
+      <c r="W9" s="75"/>
+    </row>
+    <row r="10" spans="1:23" s="117" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="84"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="67"/>
+      <c r="J10" s="67"/>
+      <c r="K10" s="67"/>
+      <c r="L10" s="68"/>
+      <c r="M10" s="69"/>
+      <c r="N10" s="70"/>
+      <c r="O10" s="71"/>
+      <c r="P10" s="72"/>
+      <c r="Q10" s="72"/>
+      <c r="R10" s="72"/>
+      <c r="S10" s="72"/>
+      <c r="T10" s="72"/>
+      <c r="U10" s="72"/>
+      <c r="V10" s="72"/>
+      <c r="W10" s="73"/>
+    </row>
+    <row r="11" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="85" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="80">
+        <f t="shared" ref="B11:W11" si="0">SUM(B8:B10)</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D11" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K11" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P11" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R11" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S11" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T11" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U11" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V11" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W11" s="39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="M6:W6"/>
+    <mergeCell ref="B6:L6"/>
+    <mergeCell ref="A2:W2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C11"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="114"/>
+    <col min="2" max="2" width="25" style="114" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="114" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="114"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="120" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="120" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B3" s="114" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="114" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B4" s="114" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="114" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="114" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="114" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="114" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="114" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="114" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="114" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="114" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="114" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="114" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="114" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="114" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="114" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="114" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="114" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>